<commit_message>
API Intergration & Config done
</commit_message>
<xml_diff>
--- a/GMU-Team 1-Requirements Traceability Matrix.xlsx
+++ b/GMU-Team 1-Requirements Traceability Matrix.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aksha_000\Documents\GitHub\gmuidt2014\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24030"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -287,7 +285,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -322,7 +320,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -499,7 +497,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -510,19 +508,19 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="78.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="78.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="28">
       <c r="A1" s="4" t="s">
         <v>35</v>
       </c>
@@ -531,7 +529,7 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -548,7 +546,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -559,13 +557,13 @@
         <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="E3" s="3">
-        <v>41651</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41662</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>2</v>
       </c>
@@ -582,7 +580,7 @@
         <v>41649</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>3</v>
       </c>
@@ -599,7 +597,7 @@
         <v>41649</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>4</v>
       </c>
@@ -616,7 +614,7 @@
         <v>41649</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>5</v>
       </c>
@@ -633,7 +631,7 @@
         <v>41649</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>6</v>
       </c>
@@ -650,7 +648,7 @@
         <v>41649</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>7</v>
       </c>
@@ -667,7 +665,7 @@
         <v>41649</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>8</v>
       </c>
@@ -684,7 +682,7 @@
         <v>41649</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>9</v>
       </c>
@@ -701,7 +699,7 @@
         <v>41649</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>10</v>
       </c>
@@ -718,7 +716,7 @@
         <v>41649</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>11</v>
       </c>
@@ -735,7 +733,7 @@
         <v>41649</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>12</v>
       </c>
@@ -746,10 +744,13 @@
         <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="E14" s="3">
+        <v>41662</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>13</v>
       </c>
@@ -763,7 +764,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>14</v>
       </c>
@@ -774,10 +775,13 @@
         <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="E16" s="3">
+        <v>41662</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>15</v>
       </c>
@@ -805,9 +809,14 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>